<commit_message>
feat: agregar boton para num_factura y cuil
</commit_message>
<xml_diff>
--- a/facturacion2.xlsx
+++ b/facturacion2.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C2"/>
+  <dimension ref="A2:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -415,6 +415,84 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>05-12-25</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>30-4567577899-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>04-12-25</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>04-12-25</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>08-12-25</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1232453</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>25323</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>512345235</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>